<commit_message>
Finally fixed bugs when optimizing for labor. Unfortunately sometimes it's not feasible at all so added brute forcing as a last resort to get results which tend towards an equilibrium point
</commit_message>
<xml_diff>
--- a/BuildingSheet.xlsx
+++ b/BuildingSheet.xlsx
@@ -699,30 +699,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -794,10 +770,10 @@
   <dimension ref="A1:CS1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.07"/>
@@ -1993,7 +1969,7 @@
         <v>99</v>
       </c>
       <c r="E5" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8" t="n">
         <v>0</v>

</xml_diff>